<commit_message>
Added vertical bars in header
</commit_message>
<xml_diff>
--- a/tests/testthat/xlsx_files/cars_no_row_names.xlsx
+++ b/tests/testthat/xlsx_files/cars_no_row_names.xlsx
@@ -151,7 +151,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -161,6 +160,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -465,7 +465,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -474,7 +474,7 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
@@ -483,27 +483,27 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="4"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="4"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>

</xml_diff>